<commit_message>
restriction of zooming feature complete
</commit_message>
<xml_diff>
--- a/documents/Coastline Generalization Testing.xlsx
+++ b/documents/Coastline Generalization Testing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7480" windowHeight="3400" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7480" windowHeight="3400" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Epsilon" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Bågø" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -16171,7 +16172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -16421,8 +16422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F1371"/>
   <sheetViews>
-    <sheetView topLeftCell="G41" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AG429" sqref="AG429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>